<commit_message>
Added indicator to AnalysisQuestions.xlsx
</commit_message>
<xml_diff>
--- a/AnalysisQuestions.xlsx
+++ b/AnalysisQuestions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\SMU\MSDS_6306_Doing_Data_Science\HW_Data\6306-case-study-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\6306\6306-case-study-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5522B6-B928-4E94-BB6B-B3067270E4E9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CDFF6884-BE40-4C33-BFFC-6EC63E820C18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17508" windowHeight="7044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17505" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
   <si>
     <t>SelfEmployed</t>
   </si>
@@ -626,27 +626,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K6" sqref="K6"/>
+      <selection pane="topRight" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.234375" customWidth="1"/>
-    <col min="4" max="4" width="20.47265625" customWidth="1"/>
-    <col min="5" max="5" width="20.234375" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.37890625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.37890625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="27.234375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="24.47265625" customWidth="1"/>
-    <col min="11" max="11" width="28.234375" customWidth="1"/>
-    <col min="12" max="12" width="19.76171875" customWidth="1"/>
+    <col min="2" max="2" width="36.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="20.25" customWidth="1"/>
+    <col min="6" max="6" width="19.875" customWidth="1"/>
+    <col min="7" max="7" width="15.375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="27.25" style="6" customWidth="1"/>
+    <col min="10" max="10" width="24.5" customWidth="1"/>
+    <col min="11" max="11" width="28.25" customWidth="1"/>
+    <col min="12" max="12" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="7" t="s">
         <v>63</v>
       </c>
@@ -666,7 +666,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>64</v>
       </c>
@@ -698,7 +698,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -709,17 +709,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>68</v>
       </c>
@@ -730,7 +730,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -741,22 +741,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -767,12 +767,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -783,7 +783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -794,12 +794,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -810,12 +810,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -826,7 +826,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -837,37 +837,37 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -881,17 +881,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -902,72 +902,72 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -978,7 +978,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -989,12 +989,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -1004,23 +1004,26 @@
       <c r="E46" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -1060,52 +1063,52 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -1116,22 +1119,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>68</v>
       </c>

</xml_diff>